<commit_message>
updates on license document
</commit_message>
<xml_diff>
--- a/Office documents/Grafice viteza_turatie.xlsx
+++ b/Office documents/Grafice viteza_turatie.xlsx
@@ -13,6 +13,20 @@
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,8 +60,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -148,23 +165,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="56657792"/>
-        <c:axId val="56659328"/>
+        <c:axId val="64853888"/>
+        <c:axId val="64855424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56657792"/>
+        <c:axId val="64853888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56659328"/>
+        <c:crossAx val="64855424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56659328"/>
+        <c:axId val="64855424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -172,20 +189,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56657792"/>
+        <c:crossAx val="64853888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -212,8 +228,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.4108772965879266"/>
-                  <c:y val="-0.66717191601049919"/>
+                  <c:x val="0.41087729658792677"/>
+                  <c:y val="-0.66717191601050008"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="#,##0.000000" sourceLinked="0"/>
@@ -365,23 +381,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="56680832"/>
-        <c:axId val="56682368"/>
+        <c:axId val="64872832"/>
+        <c:axId val="64874368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56680832"/>
+        <c:axId val="64872832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56682368"/>
+        <c:crossAx val="64874368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56682368"/>
+        <c:axId val="64874368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -389,20 +405,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56680832"/>
+        <c:crossAx val="64872832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -432,7 +447,7 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.78023600174978092"/>
+          <c:x val="0.78023600174978058"/>
           <c:y val="0.30555555555555558"/>
         </c:manualLayout>
       </c:layout>
@@ -443,9 +458,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.0599518810148754E-2"/>
+          <c:x val="7.0599518810148795E-2"/>
           <c:y val="2.8252405949256338E-2"/>
-          <c:w val="0.68243503937007899"/>
+          <c:w val="0.68243503937007932"/>
           <c:h val="0.79822506561679785"/>
         </c:manualLayout>
       </c:layout>
@@ -467,7 +482,7 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.2628926071741034"/>
+                  <c:x val="0.26289260717410357"/>
                   <c:y val="-0.64402376786235049"/>
                 </c:manualLayout>
               </c:layout>
@@ -476,7 +491,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Viteza!$A$1:$A$11</c:f>
+              <c:f>Viteza!$A$3:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -518,7 +533,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Viteza!$B$1:$B$11</c:f>
+              <c:f>Viteza!$B$3:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -560,23 +575,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="57005568"/>
-        <c:axId val="57007104"/>
+        <c:axId val="65373696"/>
+        <c:axId val="65375232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57005568"/>
+        <c:axId val="65373696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57007104"/>
+        <c:crossAx val="65375232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57007104"/>
+        <c:axId val="65375232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -584,7 +599,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57005568"/>
+        <c:crossAx val="65373696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -597,7 +612,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -612,8 +627,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.80829155730533708"/>
-          <c:y val="0.30555555555555558"/>
+          <c:x val="0.38044444444444442"/>
+          <c:y val="3.7037037037037035E-2"/>
         </c:manualLayout>
       </c:layout>
     </c:title>
@@ -625,7 +640,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Dreapta</c:v>
+            <c:v>Regresie viteza dreapta jos</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
@@ -734,23 +749,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="57172352"/>
-        <c:axId val="57173888"/>
+        <c:axId val="65413504"/>
+        <c:axId val="65415040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57172352"/>
+        <c:axId val="65413504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57173888"/>
+        <c:crossAx val="65415040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57173888"/>
+        <c:axId val="65415040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -758,7 +773,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57172352"/>
+        <c:crossAx val="65413504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -771,7 +786,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -797,10 +812,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1013495188101487"/>
+          <c:x val="0.10134951881014861"/>
           <c:y val="0.19954870224555263"/>
           <c:w val="0.50843525809273837"/>
-          <c:h val="0.65007691746864982"/>
+          <c:h val="0.65007691746865015"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -821,8 +836,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.14629330708661423"/>
-                  <c:y val="-0.62752952755905522"/>
+                  <c:x val="0.14629330708661431"/>
+                  <c:y val="-0.62752952755905556"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="0.000000000" sourceLinked="0"/>
@@ -914,23 +929,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="57194752"/>
-        <c:axId val="57208832"/>
+        <c:axId val="65435904"/>
+        <c:axId val="65441792"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57194752"/>
+        <c:axId val="65435904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57208832"/>
+        <c:crossAx val="65441792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57208832"/>
+        <c:axId val="65441792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +953,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57194752"/>
+        <c:crossAx val="65435904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -951,13 +966,188 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Regresie</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> viteza zona sus</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.5793963254593231E-2"/>
+          <c:y val="0.26899314668999691"/>
+          <c:w val="0.53501837270341213"/>
+          <c:h val="0.5621139545056868"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Regresie viteza zona sus</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.0953412073490806E-2"/>
+                  <c:y val="-0.1532524059492564"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.000000000" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Viteza!$A$40:$A$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Viteza!$B$40:$B$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>428</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>454</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>529</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="65565056"/>
+        <c:axId val="65566592"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="65565056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65566592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="65566592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65565056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -970,10 +1160,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.5793963254593176E-2"/>
-          <c:y val="0.26899314668999708"/>
-          <c:w val="0.53501837270341213"/>
-          <c:h val="0.5621139545056868"/>
+          <c:x val="0.13468285214348205"/>
+          <c:y val="0.20417833187518231"/>
+          <c:w val="0.56279615048118992"/>
+          <c:h val="0.62692876932050179"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -982,28 +1172,47 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>SUS viteza-&gt;y</c:v>
+            <c:v>Regresie viteza zona sus</c:v>
           </c:tx>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:trendline>
-            <c:trendlineType val="poly"/>
-            <c:order val="3"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="1.0953412073490813E-2"/>
-                  <c:y val="-0.15325240594925635"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="0.000000000" sourceLinked="0"/>
-            </c:trendlineLbl>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Viteza!$A$32:$A$39</c:f>
+              <c:f>Viteza!$D$49:$D$56</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>428</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>454</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>505</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>529</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Viteza!$E$49:$E$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1033,59 +1242,26 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Viteza!$B$32:$B$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>358</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>379</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>403</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>428</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>454</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>480</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>505</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>529</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="60637952"/>
-        <c:axId val="60070144"/>
+        <c:axId val="65582592"/>
+        <c:axId val="65584128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60637952"/>
+        <c:axId val="65582592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60070144"/>
+        <c:crossAx val="65584128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60070144"/>
+        <c:axId val="65584128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1093,7 +1269,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60637952"/>
+        <c:crossAx val="65582592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1106,7 +1282,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1294,6 +1470,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1589,7 +1795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1938,28 +2144,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A2:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1">
-        <v>349</v>
-      </c>
-      <c r="B1">
-        <v>0</v>
-      </c>
-    </row>
     <row r="2" spans="1:14">
-      <c r="A2">
-        <v>326</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -1974,10 +2172,10 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3">
-        <v>304</v>
+        <v>349</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L3">
         <v>10</v>
@@ -1992,10 +2190,10 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4">
-        <v>279</v>
+        <v>326</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L4">
         <v>15</v>
@@ -2010,10 +2208,10 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5">
-        <v>254</v>
+        <v>304</v>
       </c>
       <c r="B5">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="L5">
         <v>20</v>
@@ -2028,10 +2226,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6">
-        <v>230</v>
+        <v>279</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="L6">
         <v>25</v>
@@ -2046,10 +2244,10 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7">
-        <v>208</v>
+        <v>254</v>
       </c>
       <c r="B7">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="L7">
         <v>30</v>
@@ -2064,10 +2262,10 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8">
-        <v>181</v>
+        <v>230</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="L8">
         <v>34</v>
@@ -2082,10 +2280,10 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="B9">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="L9">
         <v>40</v>
@@ -2100,10 +2298,10 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10">
-        <v>136</v>
+        <v>181</v>
       </c>
       <c r="B10">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="L10">
         <v>45</v>
@@ -2118,10 +2316,10 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11">
-        <v>117</v>
+        <v>157</v>
       </c>
       <c r="B11">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="L11">
         <v>50</v>
@@ -2135,6 +2333,12 @@
       </c>
     </row>
     <row r="12" spans="1:14">
+      <c r="A12">
+        <v>136</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
       <c r="L12">
         <v>55</v>
       </c>
@@ -2146,6 +2350,22 @@
         <v>117</v>
       </c>
     </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>117</v>
+      </c>
+      <c r="B13">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="17" spans="1:2">
       <c r="A17">
         <v>112</v>
@@ -2234,73 +2454,146 @@
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32">
+    <row r="40" spans="1:5">
+      <c r="A40">
         <v>55</v>
       </c>
-      <c r="B32">
+      <c r="B40">
         <v>358</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33">
+    <row r="41" spans="1:5">
+      <c r="A41">
         <v>60</v>
       </c>
-      <c r="B33">
+      <c r="B41">
         <v>379</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
-      <c r="A34">
+    <row r="42" spans="1:5">
+      <c r="A42">
         <v>65</v>
       </c>
-      <c r="B34">
+      <c r="B42">
         <v>403</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
-      <c r="A35">
+    <row r="43" spans="1:5">
+      <c r="A43">
         <v>70</v>
       </c>
-      <c r="B35">
+      <c r="B43">
         <v>428</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36">
+    <row r="44" spans="1:5">
+      <c r="A44">
         <v>75</v>
       </c>
-      <c r="B36">
+      <c r="B44">
         <v>454</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37">
+    <row r="45" spans="1:5">
+      <c r="A45">
         <v>80</v>
       </c>
-      <c r="B37">
+      <c r="B45">
         <v>480</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38">
+    <row r="46" spans="1:5">
+      <c r="A46">
         <v>85</v>
       </c>
-      <c r="B38">
+      <c r="B46">
         <v>505</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39">
+    <row r="47" spans="1:5">
+      <c r="A47">
         <v>90</v>
       </c>
-      <c r="B39">
+      <c r="B47">
         <v>529</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="D48" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5">
+      <c r="D49">
+        <v>358</v>
+      </c>
+      <c r="E49">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="4:5">
+      <c r="D50">
+        <v>379</v>
+      </c>
+      <c r="E50">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="4:5">
+      <c r="D51">
+        <v>403</v>
+      </c>
+      <c r="E51">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="4:5">
+      <c r="D52">
+        <v>428</v>
+      </c>
+      <c r="E52">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="4:5">
+      <c r="D53">
+        <v>454</v>
+      </c>
+      <c r="E53">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="4:5">
+      <c r="D54">
+        <v>480</v>
+      </c>
+      <c r="E54">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="4:5">
+      <c r="D55">
+        <v>505</v>
+      </c>
+      <c r="E55">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="4:5">
+      <c r="D56">
+        <v>529</v>
+      </c>
+      <c r="E56">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>